<commit_message>
Updated pathway enrichment analysis and common_utils
</commit_message>
<xml_diff>
--- a/local_data/results/TableS4.xlsx
+++ b/local_data/results/TableS4.xlsx
@@ -533,16 +533,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0.0003453345225316909</v>
+        <v>0.0006906690450633818</v>
       </c>
       <c r="C2" t="s">
         <v>38</v>
       </c>
       <c r="D2">
-        <v>0.1070537019848242</v>
+        <v>0.2141074039696484</v>
       </c>
       <c r="E2">
-        <v>0.001878135122540775</v>
+        <v>0.00375627024508155</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -550,16 +550,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>1.471177039383294E-21</v>
+        <v>2.942354078766587E-21</v>
       </c>
       <c r="C3" t="s">
         <v>39</v>
       </c>
       <c r="D3">
-        <v>4.56064882208821E-19</v>
+        <v>9.12129764417642E-19</v>
       </c>
       <c r="E3">
-        <v>7.601081370147018E-20</v>
+        <v>1.520216274029404E-19</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -567,16 +567,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.001461328476475044</v>
+        <v>0.002922656952950087</v>
       </c>
       <c r="C4" t="s">
         <v>38</v>
       </c>
       <c r="D4">
-        <v>0.4530118277072636</v>
+        <v>0.9060236554145271</v>
       </c>
       <c r="E4">
-        <v>0.005807843944964918</v>
+        <v>0.01161568788992984</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -584,16 +584,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>6.340324630209424E-06</v>
+        <v>1.268064926041885E-05</v>
       </c>
       <c r="C5" t="s">
         <v>38</v>
       </c>
       <c r="D5">
-        <v>0.001965500635364921</v>
+        <v>0.003931001270729843</v>
       </c>
       <c r="E5">
-        <v>5.780884221661533E-05</v>
+        <v>0.0001156176844332307</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -601,16 +601,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>0.001979547012825534</v>
+        <v>0.003959094025651069</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
       </c>
       <c r="D6">
-        <v>0.6136595739759156</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>0.007483653341169703</v>
+        <v>0.01496730668233941</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -618,16 +618,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>0.0004486338226084451</v>
+        <v>0.0008972676452168901</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
       </c>
       <c r="D7">
-        <v>0.139076485008618</v>
+        <v>0.2781529700172359</v>
       </c>
       <c r="E7">
-        <v>0.002207563254105047</v>
+        <v>0.004415126508210094</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -635,16 +635,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>0.0005467671577189849</v>
+        <v>0.00109353431543797</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
       </c>
       <c r="D8">
-        <v>0.1694978188928853</v>
+        <v>0.3389956377857706</v>
       </c>
       <c r="E8">
-        <v>0.002576174244541352</v>
+        <v>0.005152348489082704</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -652,16 +652,16 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>0.002488275300208873</v>
+        <v>0.004976550600417746</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
       </c>
       <c r="D9">
-        <v>0.7713653430647506</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>0.009074886388997066</v>
+        <v>0.01814977277799413</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -669,16 +669,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>0.0001647304357399721</v>
+        <v>0.0003294608714799442</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
       </c>
       <c r="D10">
-        <v>0.05106643507939134</v>
+        <v>0.1021328701587827</v>
       </c>
       <c r="E10">
-        <v>0.001042172144477374</v>
+        <v>0.002084344288954749</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -686,7 +686,7 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>0.01084142624685325</v>
+        <v>0.0216828524937065</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
@@ -695,7 +695,7 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>0.03140973959368699</v>
+        <v>0.06281947918737397</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -703,16 +703,16 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>1.249825701024914E-05</v>
+        <v>2.499651402049828E-05</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
       </c>
       <c r="D12">
-        <v>0.003874459673177233</v>
+        <v>0.007748919346354466</v>
       </c>
       <c r="E12">
-        <v>0.0001076238798104787</v>
+        <v>0.0002152477596209574</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -720,16 +720,16 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>1.216711028186171E-05</v>
+        <v>2.433422056372342E-05</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
       </c>
       <c r="D13">
-        <v>0.003771804187377131</v>
+        <v>0.007543608374754262</v>
       </c>
       <c r="E13">
-        <v>0.0001076238798104787</v>
+        <v>0.0002152477596209574</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -737,7 +737,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>0.02466901902682971</v>
+        <v>0.04933803805365942</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
@@ -746,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>0.05928213874664504</v>
+        <v>0.1185642774932901</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -754,7 +754,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>0.1009637087892711</v>
+        <v>0.2019274175785423</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
@@ -763,7 +763,7 @@
         <v>1</v>
       </c>
       <c r="E15">
-        <v>0.1673729931800751</v>
+        <v>0.3347459863601502</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -771,16 +771,16 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.0001174327741957707</v>
+        <v>0.0002348655483915414</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
       </c>
       <c r="D16">
-        <v>0.03640416000068892</v>
+        <v>0.07280832000137784</v>
       </c>
       <c r="E16">
-        <v>0.00082736727274293</v>
+        <v>0.00165473454548586</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -788,16 +788,16 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>1.92992744345452E-06</v>
+        <v>3.85985488690904E-06</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
       </c>
       <c r="D17">
-        <v>0.0005982775074709013</v>
+        <v>0.001196555014941803</v>
       </c>
       <c r="E17">
-        <v>2.054388993069138E-05</v>
+        <v>4.108777986138277E-05</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -805,16 +805,16 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>0.0004182484287807559</v>
+        <v>0.0008364968575615118</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
       </c>
       <c r="D18">
-        <v>0.1296570129220343</v>
+        <v>0.2593140258440687</v>
       </c>
       <c r="E18">
-        <v>0.002125524802000562</v>
+        <v>0.004251049604001125</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -822,7 +822,7 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>0.07087739124595115</v>
+        <v>0.1417547824919023</v>
       </c>
       <c r="C19" t="s">
         <v>39</v>
@@ -831,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <v>0.1277441353851445</v>
+        <v>0.255488270770289</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -839,16 +839,16 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>0.003197156527112043</v>
+        <v>0.006394313054224087</v>
       </c>
       <c r="C20" t="s">
         <v>38</v>
       </c>
       <c r="D20">
-        <v>0.9911185234047334</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>0.01129068920235035</v>
+        <v>0.0225813784047007</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -856,16 +856,16 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>0.001919258542235698</v>
+        <v>0.003838517084471396</v>
       </c>
       <c r="C21" t="s">
         <v>38</v>
       </c>
       <c r="D21">
-        <v>0.5949701480930664</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>0.00734531047028477</v>
+        <v>0.01469062094056954</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -873,7 +873,7 @@
         <v>25</v>
       </c>
       <c r="B22">
-        <v>0.02511967463128473</v>
+        <v>0.05023934926256947</v>
       </c>
       <c r="C22" t="s">
         <v>38</v>
@@ -882,7 +882,7 @@
         <v>1</v>
       </c>
       <c r="E22">
-        <v>0.05990076258229436</v>
+        <v>0.1198015251645887</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -890,16 +890,16 @@
         <v>26</v>
       </c>
       <c r="B23">
-        <v>3.682185319492838E-57</v>
+        <v>7.364370638985677E-57</v>
       </c>
       <c r="C23" t="s">
         <v>39</v>
       </c>
       <c r="D23">
-        <v>1.14147744904278E-54</v>
+        <v>2.28295489808556E-54</v>
       </c>
       <c r="E23">
-        <v>1.14147744904278E-54</v>
+        <v>2.28295489808556E-54</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -907,16 +907,16 @@
         <v>27</v>
       </c>
       <c r="B24">
-        <v>7.06333940380206E-10</v>
+        <v>1.412667880760412E-09</v>
       </c>
       <c r="C24" t="s">
         <v>39</v>
       </c>
       <c r="D24">
-        <v>2.189635215178639E-07</v>
+        <v>4.379270430357277E-07</v>
       </c>
       <c r="E24">
-        <v>1.216464008432577E-08</v>
+        <v>2.432928016865154E-08</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -924,16 +924,16 @@
         <v>28</v>
       </c>
       <c r="B25">
-        <v>5.934028683845621E-08</v>
+        <v>1.186805736769124E-07</v>
       </c>
       <c r="C25" t="s">
         <v>39</v>
       </c>
       <c r="D25">
-        <v>1.839548891992142E-05</v>
+        <v>3.679097783984285E-05</v>
       </c>
       <c r="E25">
-        <v>8.361585872691557E-07</v>
+        <v>1.672317174538311E-06</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -941,16 +941,16 @@
         <v>29</v>
       </c>
       <c r="B26">
-        <v>1.202049205768686E-36</v>
+        <v>2.404098411537372E-36</v>
       </c>
       <c r="C26" t="s">
         <v>39</v>
       </c>
       <c r="D26">
+        <v>7.452705075765854E-34</v>
+      </c>
+      <c r="E26">
         <v>3.726352537882927E-34</v>
-      </c>
-      <c r="E26">
-        <v>1.863176268941463E-34</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -958,16 +958,16 @@
         <v>30</v>
       </c>
       <c r="B27">
-        <v>2.529407678654079E-09</v>
+        <v>5.058815357308157E-09</v>
       </c>
       <c r="C27" t="s">
         <v>39</v>
       </c>
       <c r="D27">
-        <v>7.841163803827644E-07</v>
+        <v>1.568232760765529E-06</v>
       </c>
       <c r="E27">
-        <v>4.126928317804023E-08</v>
+        <v>8.253856635608046E-08</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -975,16 +975,16 @@
         <v>31</v>
       </c>
       <c r="B28">
-        <v>5.804400457434689E-07</v>
+        <v>1.160880091486938E-06</v>
       </c>
       <c r="C28" t="s">
         <v>38</v>
       </c>
       <c r="D28">
-        <v>0.0001799364141804754</v>
+        <v>0.0003598728283609507</v>
       </c>
       <c r="E28">
-        <v>7.334168121429416E-06</v>
+        <v>1.466833624285883E-05</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -992,7 +992,7 @@
         <v>32</v>
       </c>
       <c r="B29">
-        <v>0.00434546625353703</v>
+        <v>0.00869093250707406</v>
       </c>
       <c r="C29" t="s">
         <v>39</v>
@@ -1001,7 +1001,7 @@
         <v>1</v>
       </c>
       <c r="E29">
-        <v>0.0144848875117901</v>
+        <v>0.0289697750235802</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1009,16 +1009,16 @@
         <v>33</v>
       </c>
       <c r="B30">
-        <v>3.379525317333496E-07</v>
+        <v>6.759050634666993E-07</v>
       </c>
       <c r="C30" t="s">
         <v>38</v>
       </c>
       <c r="D30">
-        <v>0.0001047652848373384</v>
+        <v>0.0002095305696746768</v>
       </c>
       <c r="E30">
-        <v>4.555012384232104E-06</v>
+        <v>9.110024768464209E-06</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1026,16 +1026,16 @@
         <v>34</v>
       </c>
       <c r="B31">
-        <v>3.306944654639802E-12</v>
+        <v>6.613889309279604E-12</v>
       </c>
       <c r="C31" t="s">
         <v>38</v>
       </c>
       <c r="D31">
-        <v>1.025152842938339E-09</v>
+        <v>2.050305685876677E-09</v>
       </c>
       <c r="E31">
-        <v>6.834352286255591E-11</v>
+        <v>1.366870457251118E-10</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1043,16 +1043,16 @@
         <v>35</v>
       </c>
       <c r="B32">
-        <v>1.489859112555306E-11</v>
+        <v>2.979718225110612E-11</v>
       </c>
       <c r="C32" t="s">
         <v>38</v>
       </c>
       <c r="D32">
-        <v>4.61856324892145E-09</v>
+        <v>9.237126497842899E-09</v>
       </c>
       <c r="E32">
-        <v>2.886602030575906E-10</v>
+        <v>5.773204061151812E-10</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1060,16 +1060,16 @@
         <v>36</v>
       </c>
       <c r="B33">
-        <v>0.002322735279642494</v>
+        <v>0.004645470559284988</v>
       </c>
       <c r="C33" t="s">
         <v>38</v>
       </c>
       <c r="D33">
-        <v>0.7200479366891731</v>
+        <v>1</v>
       </c>
       <c r="E33">
-        <v>0.008571999246299679</v>
+        <v>0.01714399849259936</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1077,7 +1077,7 @@
         <v>37</v>
       </c>
       <c r="B34">
-        <v>0.235280281115774</v>
+        <v>0.470560562231548</v>
       </c>
       <c r="C34" t="s">
         <v>39</v>
@@ -1086,7 +1086,7 @@
         <v>1</v>
       </c>
       <c r="E34">
-        <v>0.3203511140203319</v>
+        <v>0.6407022280406638</v>
       </c>
     </row>
   </sheetData>
@@ -1125,13 +1125,13 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0.1004757622416831</v>
+        <v>0.2009515244833662</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>0.2660189117863274</v>
+        <v>0.5320378235726547</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1139,13 +1139,13 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>1.444114746617082E-26</v>
+        <v>2.888229493234165E-26</v>
       </c>
       <c r="C3">
+        <v>8.953511429025911E-24</v>
+      </c>
+      <c r="D3">
         <v>4.476755714512955E-24</v>
-      </c>
-      <c r="D3">
-        <v>2.238377857256478E-24</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1153,13 +1153,13 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.2133945581570845</v>
+        <v>0.4267891163141689</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0.3556575969284742</v>
+        <v>0.7113151938569483</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1167,13 +1167,13 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>0.00249381182606931</v>
+        <v>0.00498762365213862</v>
       </c>
       <c r="C5">
-        <v>0.7730816660814861</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>0.02273769606122018</v>
+        <v>0.04547539212244036</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1181,13 +1181,13 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>0.003381662319778814</v>
+        <v>0.006763324639557628</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0.02833284646301169</v>
+        <v>0.05666569292602337</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1195,13 +1195,13 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>0.09480946607050594</v>
+        <v>0.1896189321410119</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>0.2600967653261668</v>
+        <v>0.5201935306523335</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1209,13 +1209,13 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>0.1038537209002233</v>
+        <v>0.2077074418004466</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0.2674182087888948</v>
+        <v>0.5348364175777895</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1223,13 +1223,13 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>0.06583040680128757</v>
+        <v>0.1316608136025751</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>0.2103858361690634</v>
+        <v>0.4207716723381267</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1237,13 +1237,13 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>0.1419152722902959</v>
+        <v>0.2838305445805919</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>0.311430441198408</v>
+        <v>0.622860882396816</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1251,13 +1251,13 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>0.4324533685501033</v>
+        <v>0.8649067371002066</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>0.4720441698962395</v>
+        <v>0.9440883397924791</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1265,13 +1265,13 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>0.1633968124596495</v>
+        <v>0.3267936249192991</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>0.3369200615483646</v>
+        <v>0.6738401230967292</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1279,13 +1279,13 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>0.04675328074741136</v>
+        <v>0.09350656149482271</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>0.1689029250392359</v>
+        <v>0.3378058500784719</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1293,13 +1293,13 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>0.2380730647153311</v>
+        <v>0.4761461294306623</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14">
-        <v>0.3781315177378262</v>
+        <v>0.7562630354756524</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1307,13 +1307,13 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>0.1413604939258757</v>
+        <v>0.2827209878517515</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>0.311430441198408</v>
+        <v>0.622860882396816</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1321,13 +1321,13 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.2657159636248607</v>
+        <v>0.5314319272497214</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16">
-        <v>0.3915643190011631</v>
+        <v>0.7831286380023261</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1335,13 +1335,13 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>0.09862817868195944</v>
+        <v>0.1972563573639189</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17">
-        <v>0.2636293702604146</v>
+        <v>0.5272587405208292</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1349,13 +1349,13 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>0.1970073037176554</v>
+        <v>0.3940146074353108</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18">
-        <v>0.3460012658545411</v>
+        <v>0.6920025317090821</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1363,13 +1363,13 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>0.0610343227208271</v>
+        <v>0.1220686454416542</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19">
-        <v>0.2023478654369931</v>
+        <v>0.4046957308739862</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1377,13 +1377,13 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>0.006843854004365318</v>
+        <v>0.01368770800873064</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20">
-        <v>0.0499408007216075</v>
+        <v>0.09988160144321499</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1391,13 +1391,13 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>0.4692315489175892</v>
+        <v>0.9384630978351783</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21">
-        <v>0.4887729970246832</v>
+        <v>0.9775459940493664</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1405,13 +1405,13 @@
         <v>25</v>
       </c>
       <c r="B22">
-        <v>0.1615648346388066</v>
+        <v>0.3231296692776132</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22">
-        <v>0.3369200615483646</v>
+        <v>0.6738401230967292</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1419,13 +1419,13 @@
         <v>26</v>
       </c>
       <c r="B23">
-        <v>4.641123973455231E-47</v>
+        <v>9.282247946910462E-47</v>
       </c>
       <c r="C23">
-        <v>1.438748431771121E-44</v>
+        <v>2.877496863542243E-44</v>
       </c>
       <c r="D23">
-        <v>1.438748431771121E-44</v>
+        <v>2.877496863542243E-44</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1433,13 +1433,13 @@
         <v>27</v>
       </c>
       <c r="B24">
-        <v>0.004237501295521298</v>
+        <v>0.008475002591042596</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24">
-        <v>0.03398339179318308</v>
+        <v>0.06796678358636615</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1447,13 +1447,13 @@
         <v>28</v>
       </c>
       <c r="B25">
-        <v>4.527124475152345E-06</v>
+        <v>9.05424895030469E-06</v>
       </c>
       <c r="C25">
-        <v>0.001403408587297227</v>
+        <v>0.002806817174594454</v>
       </c>
       <c r="D25">
-        <v>7.386360985774879E-05</v>
+        <v>0.0001477272197154976</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1461,13 +1461,13 @@
         <v>29</v>
       </c>
       <c r="B26">
-        <v>9.474222356466367E-17</v>
+        <v>1.894844471293273E-16</v>
       </c>
       <c r="C26">
-        <v>2.937008930504574E-14</v>
+        <v>5.874017861009147E-14</v>
       </c>
       <c r="D26">
-        <v>3.671261163130717E-15</v>
+        <v>7.342522326261434E-15</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1475,13 +1475,13 @@
         <v>30</v>
       </c>
       <c r="B27">
-        <v>3.774305290556718E-06</v>
+        <v>7.548610581113437E-06</v>
       </c>
       <c r="C27">
-        <v>0.001170034640072583</v>
+        <v>0.002340069280145165</v>
       </c>
       <c r="D27">
-        <v>6.500192444847682E-05</v>
+        <v>0.0001300038488969536</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1489,13 +1489,13 @@
         <v>31</v>
       </c>
       <c r="B28">
-        <v>0.01292675908145494</v>
+        <v>0.02585351816290988</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28">
-        <v>0.08178153704593942</v>
+        <v>0.1635630740918788</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1503,13 +1503,13 @@
         <v>32</v>
       </c>
       <c r="B29">
-        <v>0.2462923896491824</v>
+        <v>0.4925847792983649</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29">
-        <v>0.3836715617650581</v>
+        <v>0.7673431235301161</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1517,13 +1517,13 @@
         <v>33</v>
       </c>
       <c r="B30">
-        <v>0.2573141360389191</v>
+        <v>0.5146282720778381</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30">
-        <v>0.3891091813271459</v>
+        <v>0.7782183626542918</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1531,13 +1531,13 @@
         <v>34</v>
       </c>
       <c r="B31">
-        <v>0.2164621790256586</v>
+        <v>0.4329243580513171</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31">
-        <v>0.3569323164784796</v>
+        <v>0.7138646329569591</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1545,13 +1545,13 @@
         <v>35</v>
       </c>
       <c r="B32">
-        <v>0.01604755486414179</v>
+        <v>0.03209510972828358</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32">
-        <v>0.09422820848160161</v>
+        <v>0.1884564169632032</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1559,13 +1559,13 @@
         <v>36</v>
       </c>
       <c r="B33">
-        <v>0.4851834629289407</v>
+        <v>0.9703669258578814</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33">
-        <v>0.4963923218084872</v>
+        <v>0.9927846436169744</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1573,13 +1573,13 @@
         <v>37</v>
       </c>
       <c r="B34">
-        <v>0.05115818979686594</v>
+        <v>0.1023163795937319</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34">
-        <v>0.1808533233268105</v>
+        <v>0.3617066466536211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>